<commit_message>
Add ability to update performance data via admin panel
Adds a new endpoint and UI elements to the admin panel for uploading and processing the Jumbo.xlsx file, enabling updates to the performance dashboard.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 5384375e-e394-4b62-9ff7-e4b19dacf801
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 449c8bce-afa2-42a7-8237-0c92ef666d88
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d7b551d1-b37d-40c2-8d39-61fe8a04a1c4/5384375e-e394-4b62-9ff7-e4b19dacf801/TqxTvfy
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storaenso-my.sharepoint.com/personal/dariusz_buchalski_storaenso_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{2174B0B1-0BE8-4679-8D80-61363943CC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="14_{2174B0B1-0BE8-4679-8D80-61363943CC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29841A21-BAE8-40BB-B0AE-545B9C5143DE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF59FA5A-8DA5-47D9-B6C7-E39A087C6F68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF59FA5A-8DA5-47D9-B6C7-E39A087C6F68}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="9">
   <si>
     <t>Dzienne</t>
   </si>
@@ -439,8 +439,8 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:AH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,14 +580,14 @@
       <c r="I2" s="1">
         <v>717.68421052631584</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>2</v>
+      <c r="J2" s="1">
+        <v>1265.4418604651164</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2087.0270270270271</v>
+      </c>
+      <c r="L2" s="1">
+        <v>4795.3581661891121</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>2</v>
@@ -595,14 +595,14 @@
       <c r="N2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>2</v>
+      <c r="O2" s="1">
+        <v>1594.2199488491051</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2563.4862385321103</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2034.1463414634147</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>2</v>
@@ -788,8 +788,8 @@
       <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>2</v>
+      <c r="J4" s="1">
+        <v>3638</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>2</v>
@@ -893,79 +893,79 @@
         <v>717.68421052631584</v>
       </c>
       <c r="J5" s="1">
-        <v>717.68421052631584</v>
+        <v>1047.1048951048949</v>
       </c>
       <c r="K5" s="1">
-        <v>717.68421052631584</v>
+        <v>1401.7327188940094</v>
       </c>
       <c r="L5" s="1">
-        <v>717.68421052631584</v>
+        <v>2227.6569037656905</v>
       </c>
       <c r="M5" s="1">
-        <v>717.68421052631584</v>
+        <v>2227.6569037656905</v>
       </c>
       <c r="N5" s="1">
-        <v>717.68421052631584</v>
+        <v>2227.6569037656905</v>
       </c>
       <c r="O5" s="1">
-        <v>717.68421052631584</v>
+        <v>2091.9452054794519</v>
       </c>
       <c r="P5" s="1">
-        <v>717.68421052631584</v>
+        <v>2118.5211995863497</v>
       </c>
       <c r="Q5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="R5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="S5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="T5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="U5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="V5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="W5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="X5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="Y5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="Z5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AA5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AB5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AC5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AD5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AE5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AF5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AG5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
       <c r="AH5" s="1">
-        <v>717.68421052631584</v>
+        <v>2107.6181900045021</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -1100,80 +1100,80 @@
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>2</v>
+      <c r="J7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="M7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="P7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="R7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="S7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="U7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="V7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="W7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="X7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>3638</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>3638</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
@@ -1207,11 +1207,11 @@
       <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>2</v>
+      <c r="K8" s="1">
+        <v>990.26086956521749</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2762.4782608695655</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>2</v>
@@ -1225,8 +1225,8 @@
       <c r="P8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>2</v>
+      <c r="Q8" s="1">
+        <v>3221.217391304348</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>2</v>
@@ -1308,14 +1308,14 @@
       <c r="I9" s="1">
         <v>3411.2359550561796</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>2</v>
+      <c r="J9" s="1">
+        <v>3530.9774436090224</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>2</v>
+      <c r="L9" s="1">
+        <v>1923.913043478261</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>2</v>
@@ -1323,11 +1323,11 @@
       <c r="N9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>2</v>
+      <c r="O9" s="1">
+        <v>757.82608695652175</v>
+      </c>
+      <c r="P9" s="1">
+        <v>967.46606334841624</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>2</v>
@@ -1415,11 +1415,11 @@
       <c r="J10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>2</v>
+      <c r="K10" s="1">
+        <v>1125.6521739130435</v>
+      </c>
+      <c r="L10" s="1">
+        <v>815.88785046728981</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>2</v>
@@ -1427,14 +1427,14 @@
       <c r="N10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>2</v>
+      <c r="O10" s="1">
+        <v>329.92207792207796</v>
+      </c>
+      <c r="P10" s="1">
+        <v>822.67605633802816</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2763.4426229508199</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>2</v>
@@ -1520,76 +1520,76 @@
         <v>1292.8695652173915</v>
       </c>
       <c r="K11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1141.5652173913045</v>
       </c>
       <c r="L11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1681.8695652173913</v>
       </c>
       <c r="M11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1681.8695652173913</v>
       </c>
       <c r="N11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1681.8695652173913</v>
       </c>
       <c r="O11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1681.8695652173913</v>
       </c>
       <c r="P11" s="1">
-        <v>1292.8695652173915</v>
+        <v>1681.8695652173913</v>
       </c>
       <c r="Q11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="R11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="S11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="T11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="U11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="V11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="W11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="X11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="Y11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="Z11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AA11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AB11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AC11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AD11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AE11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AF11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AG11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
       <c r="AH11" s="1">
-        <v>1292.8695652173915</v>
+        <v>2066.7065217391305</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -1621,79 +1621,79 @@
         <v>3411.2359550561796</v>
       </c>
       <c r="J12" s="1">
-        <v>3411.2359550561796</v>
+        <v>3482.9729729729729</v>
       </c>
       <c r="K12" s="1">
-        <v>3411.2359550561796</v>
+        <v>3482.9729729729729</v>
       </c>
       <c r="L12" s="1">
-        <v>3411.2359550561796</v>
+        <v>2431.4076246334312</v>
       </c>
       <c r="M12" s="1">
-        <v>3411.2359550561796</v>
+        <v>2431.4076246334312</v>
       </c>
       <c r="N12" s="1">
-        <v>3411.2359550561796</v>
+        <v>2431.4076246334312</v>
       </c>
       <c r="O12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1757.2854640980738</v>
       </c>
       <c r="P12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="Q12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="R12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="S12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="T12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="U12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="V12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="W12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="X12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="Y12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="Z12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AA12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AB12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AC12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AD12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AE12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AF12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AG12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
       <c r="AH12" s="1">
-        <v>3411.2359550561796</v>
+        <v>1536.8939393939393</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -1728,76 +1728,76 @@
         <v>1044.0652173913045</v>
       </c>
       <c r="K13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1071.2608695652175</v>
       </c>
       <c r="L13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1010.8075221238938</v>
       </c>
       <c r="M13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1010.8075221238938</v>
       </c>
       <c r="N13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1010.8075221238938</v>
       </c>
       <c r="O13" s="1">
-        <v>1044.0652173913045</v>
+        <v>891.27222982216153</v>
       </c>
       <c r="P13" s="1">
-        <v>1044.0652173913045</v>
+        <v>880.11454753722785</v>
       </c>
       <c r="Q13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="R13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="S13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="T13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="U13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="V13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="W13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="X13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="Y13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="Z13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AA13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AB13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AC13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AD13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AE13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AF13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AG13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
       <c r="AH13" s="1">
-        <v>1044.0652173913045</v>
+        <v>1111.0351758793968</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -2452,14 +2452,14 @@
       <c r="I20" s="1">
         <v>2662.9565217391305</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>2</v>
+      <c r="J20" s="1">
+        <v>2862.6521739130435</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>2</v>
+      <c r="L20" s="1">
+        <v>3964.9213483146068</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>2</v>
@@ -2467,14 +2467,14 @@
       <c r="N20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>2</v>
+      <c r="O20" s="1">
+        <v>3035.739130434783</v>
+      </c>
+      <c r="P20" s="1">
+        <v>2182.695652173913</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>3279.521739130435</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>2</v>
@@ -2556,14 +2556,14 @@
       <c r="I21" s="1">
         <v>3922.434782608696</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>2</v>
+      <c r="J21" s="1">
+        <v>5705.4065934065939</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2944.2758620689656</v>
+      </c>
+      <c r="L21" s="1">
+        <v>3210.9535452322739</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>2</v>
@@ -2571,14 +2571,14 @@
       <c r="N21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>2</v>
+      <c r="O21" s="1">
+        <v>5575.4887218045105</v>
+      </c>
+      <c r="P21" s="1">
+        <v>2257.04347826087</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1753.6842105263158</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>2</v>
@@ -2660,14 +2660,14 @@
       <c r="I22" s="1">
         <v>3865.1315789473688</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>2</v>
+      <c r="J22" s="1">
+        <v>2876.2076749435664</v>
+      </c>
+      <c r="K22" s="1">
+        <v>2245.25</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1837.5652173913045</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>2</v>
@@ -2675,14 +2675,14 @@
       <c r="N22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>2</v>
+      <c r="O22" s="1">
+        <v>5148.8646288209611</v>
+      </c>
+      <c r="P22" s="1">
+        <v>3290.7189542483661</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>6743.6323851203506</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>2</v>
@@ -2765,79 +2765,79 @@
         <v>2676.4109589041095</v>
       </c>
       <c r="J23" s="1">
-        <v>2676.4109589041095</v>
+        <v>2748.4033613445381</v>
       </c>
       <c r="K23" s="1">
-        <v>2676.4109589041095</v>
+        <v>2748.4033613445381</v>
       </c>
       <c r="L23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3268.9326923076924</v>
       </c>
       <c r="M23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3268.9326923076924</v>
       </c>
       <c r="N23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3268.9326923076924</v>
       </c>
       <c r="O23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3226.7007874015753</v>
       </c>
       <c r="P23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3066.6200000000003</v>
       </c>
       <c r="Q23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="R23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="S23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="T23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="U23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="V23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="W23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="X23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="Y23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="Z23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AA23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AB23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AC23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AD23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AE23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AF23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AG23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
       <c r="AH23" s="1">
-        <v>2676.4109589041095</v>
+        <v>3094.9248554913297</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -2869,79 +2869,79 @@
         <v>4471.826086956522</v>
       </c>
       <c r="J24" s="1">
-        <v>4471.826086956522</v>
+        <v>4880.0290909090918</v>
       </c>
       <c r="K24" s="1">
-        <v>4471.826086956522</v>
+        <v>4414.8066298342546</v>
       </c>
       <c r="L24" s="1">
-        <v>4471.826086956522</v>
+        <v>4192.9157278053181</v>
       </c>
       <c r="M24" s="1">
-        <v>4471.826086956522</v>
+        <v>4192.9157278053181</v>
       </c>
       <c r="N24" s="1">
-        <v>4471.826086956522</v>
+        <v>4192.9157278053181</v>
       </c>
       <c r="O24" s="1">
-        <v>4471.826086956522</v>
+        <v>4340.9094567404427</v>
       </c>
       <c r="P24" s="1">
-        <v>4471.826086956522</v>
+        <v>4015.4159592529713</v>
       </c>
       <c r="Q24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="R24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="S24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="T24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="U24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="V24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="W24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="X24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="Y24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="Z24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AA24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AB24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AC24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AD24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AE24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AF24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AG24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
       <c r="AH24" s="1">
-        <v>4471.826086956522</v>
+        <v>3712.1670097030283</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -2973,79 +2973,79 @@
         <v>3538.7527352297593</v>
       </c>
       <c r="J25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3322.4613117170229</v>
       </c>
       <c r="K25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3040.9907457811651</v>
       </c>
       <c r="L25" s="1">
-        <v>3538.7527352297593</v>
+        <v>2799.9912929908578</v>
       </c>
       <c r="M25" s="1">
-        <v>3538.7527352297593</v>
+        <v>2799.9912929908578</v>
       </c>
       <c r="N25" s="1">
-        <v>3538.7527352297593</v>
+        <v>2799.9912929908578</v>
       </c>
       <c r="O25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3190.4754990925589</v>
       </c>
       <c r="P25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3204.7915370255137</v>
       </c>
       <c r="Q25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="R25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="S25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="T25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="U25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="V25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="W25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="X25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="Y25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="Z25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AA25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AB25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AC25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AD25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AE25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AF25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AG25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
       <c r="AH25" s="1">
-        <v>3538.7527352297593</v>
+        <v>3645.3391446472356</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
@@ -3076,14 +3076,14 @@
       <c r="I26" s="1">
         <v>1573.9565217391305</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>2</v>
+      <c r="J26" s="1">
+        <v>819.39130434782612</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1439.217391304348</v>
+      </c>
+      <c r="L26" s="1">
+        <v>2280.4719101123596</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>2</v>
@@ -3091,14 +3091,14 @@
       <c r="N26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>2</v>
+      <c r="O26" s="1">
+        <v>2858.8235294117644</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1192.0975609756099</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1400.3478260869567</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>2</v>
@@ -3180,14 +3180,14 @@
       <c r="I27" s="1">
         <v>1596.7826086956522</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>2</v>
+      <c r="J27" s="1">
+        <v>2260</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2364.8979591836733</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1738.304347826087</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>2</v>
@@ -3195,11 +3195,11 @@
       <c r="N27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>2</v>
+      <c r="O27" s="1">
+        <v>2348.6597938144328</v>
+      </c>
+      <c r="P27" s="1">
+        <v>1522.0434782608697</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>2</v>
@@ -3284,14 +3284,14 @@
       <c r="I28" s="1">
         <v>1874.1176470588236</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>2</v>
+      <c r="J28" s="1">
+        <v>2010.913043478261</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1719.6521739130435</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1594.4347826086957</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>2</v>
@@ -3299,14 +3299,14 @@
       <c r="N28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>2</v>
+      <c r="O28" s="1">
+        <v>3082.6956521739135</v>
+      </c>
+      <c r="P28" s="1">
+        <v>2890.7894736842109</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>1740.6521739130437</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>2</v>
@@ -3389,79 +3389,79 @@
         <v>1159.1379310344828</v>
       </c>
       <c r="J29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1036.2735849056603</v>
       </c>
       <c r="K29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1143.2909930715934</v>
       </c>
       <c r="L29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1529.2906178489702</v>
       </c>
       <c r="M29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1529.2906178489702</v>
       </c>
       <c r="N29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1529.2906178489702</v>
       </c>
       <c r="O29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1721.0835509138383</v>
       </c>
       <c r="P29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1658.6528497409324</v>
       </c>
       <c r="Q29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="R29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="S29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="T29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="U29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="V29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="W29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="X29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="Y29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="Z29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AA29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AB29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AC29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AD29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AE29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AF29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AG29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
       <c r="AH29" s="1">
-        <v>1159.1379310344828</v>
+        <v>1628.4494153533301</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
@@ -3493,79 +3493,79 @@
         <v>1692.1304347826087</v>
       </c>
       <c r="J30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1874.4354243542439</v>
       </c>
       <c r="K30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1994.8663697104678</v>
       </c>
       <c r="L30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1942.5531914893616</v>
       </c>
       <c r="M30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1942.5531914893616</v>
       </c>
       <c r="N30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1942.5531914893616</v>
       </c>
       <c r="O30" s="1">
-        <v>1692.1304347826087</v>
+        <v>2002.1482602118006</v>
       </c>
       <c r="P30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="Q30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="R30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="S30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="T30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="U30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="V30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="W30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="X30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="Y30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="Z30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AA30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AB30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AC30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AD30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AE30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AF30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AG30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
       <c r="AH30" s="1">
-        <v>1692.1304347826087</v>
+        <v>1930.9987113402062</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
@@ -3597,79 +3597,79 @@
         <v>1617.2523961661341</v>
       </c>
       <c r="J31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1746.6904932094353</v>
       </c>
       <c r="K31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1740</v>
       </c>
       <c r="L31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1711.1254851228978</v>
       </c>
       <c r="M31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1711.1254851228978</v>
       </c>
       <c r="N31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1711.1254851228978</v>
       </c>
       <c r="O31" s="1">
-        <v>1617.2523961661341</v>
+        <v>1938.1576106513137</v>
       </c>
       <c r="P31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2072.4389489953633</v>
       </c>
       <c r="Q31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="R31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="S31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="T31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="U31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="V31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="W31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="X31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="Y31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="Z31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AA31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AB31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AC31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AD31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AE31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AF31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AG31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
       <c r="AH31" s="1">
-        <v>1617.2523961661341</v>
+        <v>2031.1339648173207</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -3715,14 +3715,14 @@
       <c r="N32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>2</v>
+      <c r="O32" s="1">
+        <v>2355.913043478261</v>
+      </c>
+      <c r="P32" s="1">
+        <v>1360.5574912891987</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>604.77751756440273</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>2</v>
@@ -3807,11 +3807,11 @@
       <c r="J33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>2</v>
+      <c r="K33" s="1">
+        <v>1066.1224489795918</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1008.1304347826087</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>2</v>
@@ -3819,14 +3819,14 @@
       <c r="N33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>2</v>
+      <c r="O33" s="1">
+        <v>668.60869565217399</v>
+      </c>
+      <c r="P33" s="1">
+        <v>3006.8571428571427</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1386.6521739130435</v>
       </c>
       <c r="R33" s="1" t="s">
         <v>2</v>
@@ -3923,14 +3923,14 @@
       <c r="N34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>2</v>
+      <c r="O34" s="1">
+        <v>1314.3913043478262</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1273.3333333333333</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>715.82022471910113</v>
       </c>
       <c r="R34" s="1" t="s">
         <v>2</v>
@@ -4028,64 +4028,64 @@
         <v>1111.9453924914676</v>
       </c>
       <c r="O35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1539.2979835698286</v>
       </c>
       <c r="P35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1507.7490774907749</v>
       </c>
       <c r="Q35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="R35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="S35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="T35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="U35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="V35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="W35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="X35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="Y35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="Z35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AA35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AB35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AC35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AD35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AE35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AF35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AG35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
       <c r="AH35" s="1">
-        <v>1111.9453924914676</v>
+        <v>1319.9415489527521</v>
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
@@ -4120,76 +4120,76 @@
         <v>1362.8478260869567</v>
       </c>
       <c r="K36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1321.9681349578259</v>
       </c>
       <c r="L36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1227.4263261296662</v>
       </c>
       <c r="M36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1227.4263261296662</v>
       </c>
       <c r="N36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1227.4263261296662</v>
       </c>
       <c r="O36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1098.0573729240064</v>
       </c>
       <c r="P36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1431.1258828417117</v>
       </c>
       <c r="Q36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="R36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="S36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="T36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="U36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="V36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="W36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="X36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="Y36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="Z36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AA36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AB36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AC36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AD36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AE36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AF36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AG36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
       <c r="AH36" s="1">
-        <v>1362.8478260869567</v>
+        <v>1423.9902336937566</v>
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
@@ -4236,64 +4236,64 @@
         <v>1020.7526881720431</v>
       </c>
       <c r="O37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1153.4381139489196</v>
       </c>
       <c r="P37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1181.7704426106527</v>
       </c>
       <c r="Q37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="R37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="S37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="T37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="U37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="V37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="W37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="X37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="Y37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="Z37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AA37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AB37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AC37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AD37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AE37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AF37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AG37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
       <c r="AH37" s="1">
-        <v>1020.7526881720431</v>
+        <v>1065.1518560179979</v>
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
@@ -4324,14 +4324,14 @@
       <c r="I38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>2</v>
+      <c r="J38" s="1">
+        <v>2006.608695652174</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1183.0434782608697</v>
+      </c>
+      <c r="L38" s="1">
+        <v>820.43126684636127</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>2</v>
@@ -4339,11 +4339,11 @@
       <c r="N38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>2</v>
+      <c r="O38" s="1">
+        <v>1900.9756097560976</v>
+      </c>
+      <c r="P38" s="1">
+        <v>816.00000000000011</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>2</v>
@@ -4428,11 +4428,11 @@
       <c r="I39" s="1">
         <v>3507.7611940298507</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>2</v>
+      <c r="J39" s="1">
+        <v>2986.2857142857142</v>
+      </c>
+      <c r="K39" s="1">
+        <v>1529.4782608695652</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>2</v>
@@ -4443,14 +4443,14 @@
       <c r="N39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>2</v>
+      <c r="O39" s="1">
+        <v>780.41379310344826</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q39" s="1" t="s">
-        <v>2</v>
+      <c r="Q39" s="1">
+        <v>1091.3478260869565</v>
       </c>
       <c r="R39" s="1" t="s">
         <v>2</v>
@@ -4535,8 +4535,8 @@
       <c r="J40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>2</v>
+      <c r="K40" s="1">
+        <v>2091.818181818182</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>2</v>
@@ -4547,14 +4547,14 @@
       <c r="N40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>2</v>
+      <c r="O40" s="1">
+        <v>1747.8202247191011</v>
+      </c>
+      <c r="P40" s="1">
+        <v>950.78260869565213</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>1002.2608695652175</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>2</v>
@@ -4637,79 +4637,79 @@
         <v>2660.8695652173915</v>
       </c>
       <c r="J41" s="1">
-        <v>2660.8695652173915</v>
+        <v>2333.739130434783</v>
       </c>
       <c r="K41" s="1">
-        <v>2660.8695652173915</v>
+        <v>2103.6000000000004</v>
       </c>
       <c r="L41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1790.6114398422092</v>
       </c>
       <c r="M41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1790.6114398422092</v>
       </c>
       <c r="N41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1790.6114398422092</v>
       </c>
       <c r="O41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1815.8519269776875</v>
       </c>
       <c r="P41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="Q41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="R41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="S41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="T41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="U41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="V41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="W41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="X41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="Y41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="Z41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AA41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AB41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AC41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AD41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AE41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AF41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AG41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
       <c r="AH41" s="1">
-        <v>2660.8695652173915</v>
+        <v>1626.735197368421</v>
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
@@ -4741,79 +4741,79 @@
         <v>2808.0933852140079</v>
       </c>
       <c r="J42" s="1">
-        <v>2808.0933852140079</v>
+        <v>2859.779005524862</v>
       </c>
       <c r="K42" s="1">
-        <v>2808.0933852140079</v>
+        <v>2342.9391891891892</v>
       </c>
       <c r="L42" s="1">
-        <v>2808.0933852140079</v>
+        <v>2342.9391891891892</v>
       </c>
       <c r="M42" s="1">
-        <v>2808.0933852140079</v>
+        <v>2342.9391891891892</v>
       </c>
       <c r="N42" s="1">
-        <v>2808.0933852140079</v>
+        <v>2342.9391891891892</v>
       </c>
       <c r="O42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1923.1130327362571</v>
       </c>
       <c r="P42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1923.1130327362571</v>
       </c>
       <c r="Q42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="R42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="S42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="T42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="U42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="V42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="W42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="X42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="Y42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="Z42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AA42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AB42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AC42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AD42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AE42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AF42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AG42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
       <c r="AH42" s="1">
-        <v>2808.0933852140079</v>
+        <v>1739.0764790764792</v>
       </c>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
@@ -4847,77 +4847,77 @@
       <c r="J43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="X43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH43" s="1" t="s">
-        <v>2</v>
+      <c r="K43" s="1">
+        <v>2091.818181818182</v>
+      </c>
+      <c r="L43" s="1">
+        <v>2091.818181818182</v>
+      </c>
+      <c r="M43" s="1">
+        <v>2091.818181818182</v>
+      </c>
+      <c r="N43" s="1">
+        <v>2091.818181818182</v>
+      </c>
+      <c r="O43" s="1">
+        <v>1804.6153846153848</v>
+      </c>
+      <c r="P43" s="1">
+        <v>1469.1116173120727</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="R43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="S43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="T43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="U43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="V43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="W43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="X43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AF43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AG43" s="1">
+        <v>1308.6098654708519</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>1308.6098654708519</v>
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
@@ -4948,14 +4948,14 @@
       <c r="I44" s="1">
         <v>3779.8648648648646</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>2</v>
+      <c r="J44" s="1">
+        <v>6781.3422818791942</v>
+      </c>
+      <c r="K44" s="1">
+        <v>5193.4851936218674</v>
+      </c>
+      <c r="L44" s="1">
+        <v>3386.2753950338597</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>2</v>
@@ -4963,14 +4963,14 @@
       <c r="N44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>2</v>
+      <c r="O44" s="1">
+        <v>5067.2359550561796</v>
+      </c>
+      <c r="P44" s="1">
+        <v>4757.0984455958551</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>9520.8695652173901</v>
       </c>
       <c r="R44" s="1" t="s">
         <v>2</v>
@@ -5052,14 +5052,14 @@
       <c r="I45" s="1">
         <v>4524.9655172413795</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>2</v>
+      <c r="J45" s="1">
+        <v>4130.086956521739</v>
+      </c>
+      <c r="K45" s="1">
+        <v>3089.318181818182</v>
+      </c>
+      <c r="L45" s="1">
+        <v>971.86363636363626</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>2</v>
@@ -5067,14 +5067,14 @@
       <c r="N45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>2</v>
+      <c r="O45" s="1">
+        <v>4021.7777777777778</v>
+      </c>
+      <c r="P45" s="1">
+        <v>5971.5652173913049</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>4064.2035398230091</v>
       </c>
       <c r="R45" s="1" t="s">
         <v>2</v>
@@ -5156,14 +5156,14 @@
       <c r="I46" s="1">
         <v>3441.8426966292132</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>2</v>
+      <c r="J46" s="1">
+        <v>4516.3274336283184</v>
+      </c>
+      <c r="K46" s="1">
+        <v>4550.217391304348</v>
+      </c>
+      <c r="L46" s="1">
+        <v>3692.1379310344828</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>2</v>
@@ -5171,14 +5171,14 @@
       <c r="N46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>2</v>
+      <c r="O46" s="1">
+        <v>5901.8426966292136</v>
+      </c>
+      <c r="P46" s="1">
+        <v>5746.3829787234044</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>5455.0714285714284</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>2</v>
@@ -5261,79 +5261,79 @@
         <v>2250.2238805970151</v>
       </c>
       <c r="J47" s="1">
-        <v>2250.2238805970151</v>
+        <v>3869.2565947242206</v>
       </c>
       <c r="K47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4213.2426035502958</v>
       </c>
       <c r="L47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4041.4908579465537</v>
       </c>
       <c r="M47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4041.4908579465537</v>
       </c>
       <c r="N47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4041.4908579465537</v>
       </c>
       <c r="O47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4218.5492629945693</v>
       </c>
       <c r="P47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4288.6842105263149</v>
       </c>
       <c r="Q47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="R47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="S47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="T47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="U47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="V47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="W47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="X47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="Y47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="Z47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AA47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AB47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AC47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AD47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AE47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AF47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AG47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
       <c r="AH47" s="1">
-        <v>2250.2238805970151</v>
+        <v>4521.4506769825912</v>
       </c>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
@@ -5365,79 +5365,79 @@
         <v>4116.2711864406783</v>
       </c>
       <c r="J48" s="1">
-        <v>4116.2711864406783</v>
+        <v>4120.9962825278817</v>
       </c>
       <c r="K48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3907.0005892751919</v>
       </c>
       <c r="L48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3302.667290594291</v>
       </c>
       <c r="M48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3302.667290594291</v>
       </c>
       <c r="N48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3302.667290594291</v>
       </c>
       <c r="O48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3417.2383949645946</v>
       </c>
       <c r="P48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3808.6409060626252</v>
       </c>
       <c r="Q48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="R48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="S48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="T48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="U48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="V48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="W48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="X48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="Y48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="Z48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AA48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AB48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AC48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AD48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AE48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AF48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AG48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
       <c r="AH48" s="1">
-        <v>4116.2711864406783</v>
+        <v>3842.0845396641571</v>
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
@@ -5469,79 +5469,79 @@
         <v>2956.3820224719102</v>
       </c>
       <c r="J49" s="1">
-        <v>2956.3820224719102</v>
+        <v>3481.7883755588673</v>
       </c>
       <c r="K49" s="1">
-        <v>2956.3820224719102</v>
+        <v>3754.5283018867926</v>
       </c>
       <c r="L49" s="1">
-        <v>2956.3820224719102</v>
+        <v>3742.3960661600358</v>
       </c>
       <c r="M49" s="1">
-        <v>2956.3820224719102</v>
+        <v>3742.3960661600358</v>
       </c>
       <c r="N49" s="1">
-        <v>2956.3820224719102</v>
+        <v>3742.3960661600358</v>
       </c>
       <c r="O49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4100.6935123042513</v>
       </c>
       <c r="P49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4257.2672064777335</v>
       </c>
       <c r="Q49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="R49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="S49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="T49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="U49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="V49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="W49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="X49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="Y49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="Z49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AA49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AB49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AC49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AD49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AE49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AF49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AG49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
       <c r="AH49" s="1">
-        <v>2956.3820224719102</v>
+        <v>4360.653514180025</v>
       </c>
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
@@ -5572,14 +5572,14 @@
       <c r="I50" s="1">
         <v>2848.826086956522</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>2</v>
+      <c r="J50" s="1">
+        <v>3153.2608695652175</v>
+      </c>
+      <c r="K50" s="1">
+        <v>7732.3043478260879</v>
+      </c>
+      <c r="L50" s="1">
+        <v>11449.846153846154</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>2</v>
@@ -5587,14 +5587,14 @@
       <c r="N50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>2</v>
+      <c r="O50" s="1">
+        <v>1891.7468354430378</v>
+      </c>
+      <c r="P50" s="1">
+        <v>9879.7350993377477</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>12177.272727272728</v>
       </c>
       <c r="R50" s="1" t="s">
         <v>2</v>
@@ -5676,14 +5676,14 @@
       <c r="I51" s="1">
         <v>11250.663716814159</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>2</v>
+      <c r="J51" s="1">
+        <v>11467</v>
+      </c>
+      <c r="K51" s="1">
+        <v>10638</v>
+      </c>
+      <c r="L51" s="1">
+        <v>5296.8396226415098</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>2</v>
@@ -5694,11 +5694,11 @@
       <c r="O51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>2</v>
+      <c r="P51" s="1">
+        <v>4106.8965517241377</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>3208.6956521739135</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>2</v>
@@ -5780,11 +5780,11 @@
       <c r="I52" s="1">
         <v>2743.5652173913045</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>2</v>
+      <c r="J52" s="1">
+        <v>4833.2608695652179</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3209.0526315789471</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>2</v>
@@ -5798,11 +5798,11 @@
       <c r="O52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>2</v>
+      <c r="P52" s="1">
+        <v>3588.6</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>3138.7775061124694</v>
       </c>
       <c r="R52" s="1" t="s">
         <v>2</v>
@@ -5885,79 +5885,79 @@
         <v>2848.826086956522</v>
       </c>
       <c r="J53" s="1">
-        <v>2848.826086956522</v>
+        <v>3001.04347826087</v>
       </c>
       <c r="K53" s="1">
-        <v>2848.826086956522</v>
+        <v>4578.130434782609</v>
       </c>
       <c r="L53" s="1">
-        <v>2848.826086956522</v>
+        <v>6092.2372881355941</v>
       </c>
       <c r="M53" s="1">
-        <v>2848.826086956522</v>
+        <v>6092.2372881355941</v>
       </c>
       <c r="N53" s="1">
-        <v>2848.826086956522</v>
+        <v>6092.2372881355941</v>
       </c>
       <c r="O53" s="1">
-        <v>2848.826086956522</v>
+        <v>5325.8660508083149</v>
       </c>
       <c r="P53" s="1">
-        <v>2848.826086956522</v>
+        <v>6113.8349885408707</v>
       </c>
       <c r="Q53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="R53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="S53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="T53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="U53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="V53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="W53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="X53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="Y53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="Z53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AA53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AB53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AC53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AD53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AE53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AF53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AG53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
       <c r="AH53" s="1">
-        <v>2848.826086956522</v>
+        <v>6495.7838224767365</v>
       </c>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
@@ -5989,79 +5989,79 @@
         <v>11250.663716814159</v>
       </c>
       <c r="J54" s="1">
-        <v>11250.663716814159</v>
+        <v>11362.081545064379</v>
       </c>
       <c r="K54" s="1">
-        <v>11250.663716814159</v>
+        <v>11115.934844192636</v>
       </c>
       <c r="L54" s="1">
-        <v>11250.663716814159</v>
+        <v>9772.091503267975</v>
       </c>
       <c r="M54" s="1">
-        <v>11250.663716814159</v>
+        <v>9772.091503267975</v>
       </c>
       <c r="N54" s="1">
-        <v>11250.663716814159</v>
+        <v>9772.091503267975</v>
       </c>
       <c r="O54" s="1">
-        <v>11250.663716814159</v>
+        <v>9772.091503267975</v>
       </c>
       <c r="P54" s="1">
-        <v>11250.663716814159</v>
+        <v>9684</v>
       </c>
       <c r="Q54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="R54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="S54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="T54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="U54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="V54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="W54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="X54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="Y54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="Z54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AA54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AB54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AC54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AD54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AE54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AF54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AG54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
       <c r="AH54" s="1">
-        <v>11250.663716814159</v>
+        <v>8402.8645161290315</v>
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
@@ -6093,79 +6093,79 @@
         <v>6202.265060240964</v>
       </c>
       <c r="J55" s="1">
-        <v>6202.265060240964</v>
+        <v>5714.0930232558139</v>
       </c>
       <c r="K55" s="1">
-        <v>6202.265060240964</v>
+        <v>5144.08383233533</v>
       </c>
       <c r="L55" s="1">
-        <v>6202.265060240964</v>
+        <v>5144.08383233533</v>
       </c>
       <c r="M55" s="1">
-        <v>6202.265060240964</v>
+        <v>5144.08383233533</v>
       </c>
       <c r="N55" s="1">
-        <v>6202.265060240964</v>
+        <v>5144.08383233533</v>
       </c>
       <c r="O55" s="1">
-        <v>6202.265060240964</v>
+        <v>5144.08383233533</v>
       </c>
       <c r="P55" s="1">
-        <v>6202.265060240964</v>
+        <v>4843.507246376812</v>
       </c>
       <c r="Q55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="R55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="S55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="T55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="U55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="V55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="W55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="X55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="Y55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="Z55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AA55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AB55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AC55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AD55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AE55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AF55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AG55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
       <c r="AH55" s="1">
-        <v>6202.265060240964</v>
+        <v>4562.2509076240422</v>
       </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
@@ -6196,14 +6196,14 @@
       <c r="I56" s="1">
         <v>1761.1304347826087</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>2</v>
+      <c r="J56" s="1">
+        <v>1932.7826086956522</v>
+      </c>
+      <c r="K56" s="1">
+        <v>3673.6956521739135</v>
+      </c>
+      <c r="L56" s="1">
+        <v>2637.6053215077604</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>2</v>
@@ -6211,14 +6211,14 @@
       <c r="N56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>2</v>
+      <c r="O56" s="1">
+        <v>1469.3478260869567</v>
+      </c>
+      <c r="P56" s="1">
+        <v>2613.2608695652175</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>696</v>
       </c>
       <c r="R56" s="1" t="s">
         <v>2</v>
@@ -6300,14 +6300,14 @@
       <c r="I57" s="1">
         <v>2159.3406593406594</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>2</v>
+      <c r="J57" s="1">
+        <v>3178.7412587412587</v>
+      </c>
+      <c r="K57" s="1">
+        <v>3142.5333333333333</v>
+      </c>
+      <c r="L57" s="1">
+        <v>3431.4782608695655</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>2</v>
@@ -6318,11 +6318,11 @@
       <c r="O57" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>2</v>
+      <c r="P57" s="1">
+        <v>3007.826086956522</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>2926.304347826087</v>
       </c>
       <c r="R57" s="1" t="s">
         <v>2</v>
@@ -6404,14 +6404,14 @@
       <c r="I58" s="1">
         <v>3926.5771812080534</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>2</v>
+      <c r="J58" s="1">
+        <v>3601.9292604501607</v>
+      </c>
+      <c r="K58" s="1">
+        <v>3561.3913043478265</v>
+      </c>
+      <c r="L58" s="1">
+        <v>3474.2769230769227</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>2</v>
@@ -6509,79 +6509,79 @@
         <v>2421.326086956522</v>
       </c>
       <c r="J59" s="1">
-        <v>2421.326086956522</v>
+        <v>2258.478260869565</v>
       </c>
       <c r="K59" s="1">
-        <v>2421.326086956522</v>
+        <v>2612.2826086956525</v>
       </c>
       <c r="L59" s="1">
-        <v>2421.326086956522</v>
+        <v>2617.2675687472715</v>
       </c>
       <c r="M59" s="1">
-        <v>2421.326086956522</v>
+        <v>2617.2675687472715</v>
       </c>
       <c r="N59" s="1">
-        <v>2421.326086956522</v>
+        <v>2617.2675687472715</v>
       </c>
       <c r="O59" s="1">
-        <v>2421.326086956522</v>
+        <v>2425.3217011995639</v>
       </c>
       <c r="P59" s="1">
-        <v>2421.326086956522</v>
+        <v>2452.2454064154467</v>
       </c>
       <c r="Q59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="R59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="S59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="T59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="U59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="V59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="W59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="X59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="Y59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="Z59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AA59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AB59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AC59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AD59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AE59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AF59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AG59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
       <c r="AH59" s="1">
-        <v>2421.326086956522</v>
+        <v>2232.1765186597654</v>
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.25">
@@ -6613,79 +6613,79 @@
         <v>2965.216316440049</v>
       </c>
       <c r="J60" s="1">
-        <v>2965.216316440049</v>
+        <v>2997.2899159663866</v>
       </c>
       <c r="K60" s="1">
-        <v>2965.216316440049</v>
+        <v>3043.9087018544933</v>
       </c>
       <c r="L60" s="1">
-        <v>2965.216316440049</v>
+        <v>3139.6562835660579</v>
       </c>
       <c r="M60" s="1">
-        <v>2965.216316440049</v>
+        <v>3139.6562835660579</v>
       </c>
       <c r="N60" s="1">
-        <v>2965.216316440049</v>
+        <v>3139.6562835660579</v>
       </c>
       <c r="O60" s="1">
-        <v>2965.216316440049</v>
+        <v>3139.6562835660579</v>
       </c>
       <c r="P60" s="1">
-        <v>2965.216316440049</v>
+        <v>3113.5400516795862</v>
       </c>
       <c r="Q60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="R60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="S60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="T60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="U60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="V60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="W60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="X60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="Y60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="Z60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AA60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AB60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AC60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AD60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AE60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AF60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AG60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
       <c r="AH60" s="1">
-        <v>2965.216316440049</v>
+        <v>3082.5808770668582</v>
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.25">
@@ -6717,79 +6717,79 @@
         <v>3070.6504961411247</v>
       </c>
       <c r="J61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3206.3054187192115</v>
       </c>
       <c r="K61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3303.6471990464838</v>
       </c>
       <c r="L61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="M61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="N61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="O61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="P61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="Q61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="R61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="S61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="T61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="U61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="V61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="W61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="X61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="Y61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="Z61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AA61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AB61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AC61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AD61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AE61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AF61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AG61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
       <c r="AH61" s="1">
-        <v>3070.6504961411247</v>
+        <v>3331.3330004992513</v>
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
@@ -6820,14 +6820,14 @@
       <c r="I62" s="1">
         <v>3888.3913043478265</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>2</v>
+      <c r="J62" s="1">
+        <v>5528.1222707423585</v>
+      </c>
+      <c r="K62" s="1">
+        <v>4510.1739130434789</v>
+      </c>
+      <c r="L62" s="1">
+        <v>7733.3447098976121</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>2</v>
@@ -6835,14 +6835,14 @@
       <c r="N62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>2</v>
+      <c r="O62" s="1">
+        <v>2748.3116883116886</v>
+      </c>
+      <c r="P62" s="1">
+        <v>3525.9060402684563</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>3890.5909090909086</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>2</v>
@@ -6924,14 +6924,14 @@
       <c r="I63" s="1">
         <v>3437.8666666666668</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>2</v>
+      <c r="J63" s="1">
+        <v>2608.434782608696</v>
+      </c>
+      <c r="K63" s="1">
+        <v>3376.304347826087</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1982.608695652174</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>2</v>
@@ -6942,11 +6942,11 @@
       <c r="O63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>2</v>
+      <c r="P63" s="1">
+        <v>1509.4090909090908</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>7305.875</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>2</v>
@@ -7028,14 +7028,14 @@
       <c r="I64" s="1">
         <v>6810.4677060133627</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>2</v>
+      <c r="J64" s="1">
+        <v>13041.842696629214</v>
+      </c>
+      <c r="K64" s="1">
+        <v>3717.8426966292132</v>
+      </c>
+      <c r="L64" s="1">
+        <v>5009.333333333333</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>2</v>
@@ -7043,14 +7043,14 @@
       <c r="N64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P64" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q64" s="1" t="s">
-        <v>2</v>
+      <c r="O64" s="1">
+        <v>10182.857142857143</v>
+      </c>
+      <c r="P64" s="1">
+        <v>6220.5842696629215</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>5994</v>
       </c>
       <c r="R64" s="1" t="s">
         <v>2</v>
@@ -7133,79 +7133,79 @@
         <v>3888.3913043478265</v>
       </c>
       <c r="J65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4706.4705882352946</v>
       </c>
       <c r="K65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4640.9433962264156</v>
       </c>
       <c r="L65" s="1">
-        <v>3888.3913043478265</v>
+        <v>5563.6252545824846</v>
       </c>
       <c r="M65" s="1">
-        <v>3888.3913043478265</v>
+        <v>5563.6252545824846</v>
       </c>
       <c r="N65" s="1">
-        <v>3888.3913043478265</v>
+        <v>5563.6252545824846</v>
       </c>
       <c r="O65" s="1">
-        <v>3888.3913043478265</v>
+        <v>5102.1966794380578</v>
       </c>
       <c r="P65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4850.1931330472098</v>
       </c>
       <c r="Q65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="R65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="S65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="T65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="U65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="V65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="W65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="X65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="Y65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="Z65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AA65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AB65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AC65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AD65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AE65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AF65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AG65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
       <c r="AH65" s="1">
-        <v>3888.3913043478265</v>
+        <v>4719.7156983930772</v>
       </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.25">
@@ -7237,79 +7237,79 @@
         <v>3436.5405405405409</v>
       </c>
       <c r="J66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3119.1</v>
       </c>
       <c r="K66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3190.3734939759038</v>
       </c>
       <c r="L66" s="1">
-        <v>3436.5405405405409</v>
+        <v>2928.3113207547176</v>
       </c>
       <c r="M66" s="1">
-        <v>3436.5405405405409</v>
+        <v>2928.3113207547176</v>
       </c>
       <c r="N66" s="1">
-        <v>3436.5405405405409</v>
+        <v>2928.3113207547176</v>
       </c>
       <c r="O66" s="1">
-        <v>3436.5405405405409</v>
+        <v>2928.3113207547176</v>
       </c>
       <c r="P66" s="1">
-        <v>3436.5405405405409</v>
+        <v>2684.4375</v>
       </c>
       <c r="Q66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="R66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="S66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="T66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="U66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="V66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="W66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="X66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="Y66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="Z66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AA66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AB66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AC66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AD66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AE66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AF66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AG66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
       <c r="AH66" s="1">
-        <v>3436.5405405405409</v>
+        <v>3414.1381578947367</v>
       </c>
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.25">
@@ -7341,79 +7341,79 @@
         <v>4785.8085808580863</v>
       </c>
       <c r="J67" s="1">
-        <v>4785.8085808580863</v>
+        <v>7499.2023633677991</v>
       </c>
       <c r="K67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6563.8465814341307</v>
       </c>
       <c r="L67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6252.8056914184081</v>
       </c>
       <c r="M67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6252.8056914184081</v>
       </c>
       <c r="N67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6252.8056914184081</v>
       </c>
       <c r="O67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6905.6284760845392</v>
       </c>
       <c r="P67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6808.605983450032</v>
       </c>
       <c r="Q67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="R67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="S67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="T67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="U67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="V67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="W67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="X67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="Y67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="Z67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AA67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AB67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AC67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AD67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AE67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AF67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AG67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
       <c r="AH67" s="1">
-        <v>4785.8085808580863</v>
+        <v>6706.5534521158124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>